<commit_message>
feat: user form component created
It has also been fixed the problem with excels actualization
</commit_message>
<xml_diff>
--- a/excels/respuestas_formulario2.xlsx
+++ b/excels/respuestas_formulario2.xlsx
@@ -158,7 +158,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AH2"/>
+  <dimension ref="A1:AH4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -276,7 +276,7 @@
         <v>1.0</v>
       </c>
       <c r="C2" t="n" s="0">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D2" t="n" s="0">
         <v>0.0</v>
@@ -369,6 +369,214 @@
         <v>0.0</v>
       </c>
       <c r="AH2" t="n" s="0">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="B3" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="C3" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="D3" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E3" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="F3" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G3" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="H3" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="I3" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="J3" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K3" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="L3" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M3" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="N3" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O3" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="P3" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="Q3" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="R3" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="S3" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="T3" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="U3" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="V3" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="W3" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="X3" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Y3" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="Z3" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="AA3" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AB3" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="AC3" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AD3" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="AE3" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="AF3" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="AG3" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AH3" t="n" s="0">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="B4" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="C4" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="D4" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E4" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="F4" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="G4" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="H4" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="I4" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="J4" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K4" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="L4" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M4" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="N4" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O4" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="P4" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="Q4" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="R4" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="S4" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="T4" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="U4" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="V4" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="W4" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="X4" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Y4" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="Z4" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="AA4" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AB4" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="AC4" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AD4" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="AE4" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="AF4" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="AG4" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AH4" t="n" s="0">
         <v>1.0</v>
       </c>
     </row>

</xml_diff>